<commit_message>
ran acinetobacter again with code updates. user no longer has to specify orthology data
</commit_message>
<xml_diff>
--- a/indigoData/acinetobacter.xlsx
+++ b/indigoData/acinetobacter.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2610" uniqueCount="6">
   <si>
     <t>AMK</t>
   </si>
@@ -73,7 +73,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -85,16 +85,120 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,10 +1036,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -943,10 +1047,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="55" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -954,10 +1058,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -965,10 +1069,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -976,10 +1080,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -987,10 +1091,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="55" t="s">
         <v>2</v>
       </c>
       <c r="C6">
@@ -998,10 +1102,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C7">
@@ -1009,10 +1113,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C8">
@@ -1020,10 +1124,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C9">
@@ -1031,10 +1135,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C10">
@@ -1042,10 +1146,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C11">
@@ -1053,10 +1157,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C12">
@@ -1064,10 +1168,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C13">
@@ -1075,10 +1179,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C14">
@@ -1086,10 +1190,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C15">
@@ -1097,10 +1201,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="55" t="s">
         <v>1</v>
       </c>
       <c r="C16">
@@ -1108,10 +1212,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="55" t="s">
         <v>2</v>
       </c>
       <c r="C17">
@@ -1119,10 +1223,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C18">
@@ -1130,10 +1234,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C19">
@@ -1141,10 +1245,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C20">
@@ -1152,10 +1256,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="55" t="s">
         <v>2</v>
       </c>
       <c r="C21">
@@ -1163,10 +1267,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C22">
@@ -1174,10 +1278,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C23">
@@ -1185,10 +1289,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C24">
@@ -1196,10 +1300,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C25">
@@ -1207,10 +1311,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C26">
@@ -1218,10 +1322,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C27">
@@ -1229,10 +1333,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C28">
@@ -1240,10 +1344,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C29">
@@ -1251,10 +1355,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="A30" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C30">
@@ -1262,10 +1366,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="A31" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="55" t="s">
         <v>1</v>
       </c>
       <c r="C31">
@@ -1273,10 +1377,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="A32" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="55" t="s">
         <v>2</v>
       </c>
       <c r="C32">
@@ -1284,10 +1388,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C33">
@@ -1295,10 +1399,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="A34" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C34">
@@ -1306,10 +1410,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="A35" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C35">
@@ -1317,10 +1421,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="A36" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="55" t="s">
         <v>2</v>
       </c>
       <c r="C36">
@@ -1328,10 +1432,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C37">
@@ -1339,10 +1443,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="A38" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C38">
@@ -1350,10 +1454,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C39">
@@ -1361,10 +1465,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="3" t="s">
+      <c r="A40" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C40">
@@ -1372,10 +1476,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C41">
@@ -1383,10 +1487,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="A42" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C42">
@@ -1394,10 +1498,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="3" t="s">
+      <c r="A43" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C43">
@@ -1405,10 +1509,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="A44" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C44">
@@ -1416,10 +1520,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="3" t="s">
+      <c r="A45" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C45">

</xml_diff>